<commit_message>
Fixed Employee Count Bug
</commit_message>
<xml_diff>
--- a/Outputs/Test List.xlsx
+++ b/Outputs/Test List.xlsx
@@ -564,14 +564,14 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>$175,637.81</t>
+          <t>$381,558.00</t>
         </is>
       </c>
       <c r="G2" t="n">
         <v>4.611689712830751</v>
       </c>
       <c r="H2" t="n">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
@@ -638,14 +638,14 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>$164,243.46</t>
+          <t>$356,804.76</t>
         </is>
       </c>
       <c r="G3" t="n">
         <v>2.475442282836417</v>
       </c>
       <c r="H3" t="n">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
@@ -712,14 +712,14 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>$178,941.12</t>
+          <t>$346,337.65</t>
         </is>
       </c>
       <c r="G4" t="n">
         <v>2.664917798378182</v>
       </c>
       <c r="H4" t="n">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
@@ -786,14 +786,14 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>$178,160.92</t>
+          <t>$349,723.30</t>
         </is>
       </c>
       <c r="G5" t="n">
         <v>2.987038853679983</v>
       </c>
       <c r="H5" t="n">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
@@ -860,14 +860,14 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>$169,000.15</t>
+          <t>$338,000.30</t>
         </is>
       </c>
       <c r="G6" t="n">
         <v>5.942787141979275</v>
       </c>
       <c r="H6" t="n">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
@@ -934,14 +934,14 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$182,967.22</t>
+          <t>$351,860.04</t>
         </is>
       </c>
       <c r="G7" t="n">
         <v>4.441620307725067</v>
       </c>
       <c r="H7" t="n">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="I7" t="n">
         <v>1</v>
@@ -1008,14 +1008,14 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>$166,855.72</t>
+          <t>$333,711.44</t>
         </is>
       </c>
       <c r="G8" t="n">
         <v>1.48533491287494</v>
       </c>
       <c r="H8" t="n">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
@@ -1082,14 +1082,14 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>$154,768.69</t>
+          <t>$315,269.56</t>
         </is>
       </c>
       <c r="G9" t="n">
         <v>3.986449103283516</v>
       </c>
       <c r="H9" t="n">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
@@ -1156,14 +1156,14 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>$156,988.46</t>
+          <t>$301,900.88</t>
         </is>
       </c>
       <c r="G10" t="n">
         <v>3.367337318934143</v>
       </c>
       <c r="H10" t="n">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
@@ -1230,14 +1230,14 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>$177,885.33</t>
+          <t>$449,394.53</t>
         </is>
       </c>
       <c r="G11" t="n">
         <v>-0.07315691194327432</v>
       </c>
       <c r="H11" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
@@ -1304,14 +1304,14 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>$149,100.25</t>
+          <t>$397,600.67</t>
         </is>
       </c>
       <c r="G12" t="n">
         <v>-0.05053339391896839</v>
       </c>
       <c r="H12" t="n">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="I12" t="n">
         <v>1</v>
@@ -1378,14 +1378,14 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>$175,711.54</t>
+          <t>$496,126.71</t>
         </is>
       </c>
       <c r="G13" t="n">
         <v>-0.7630106113784501</v>
       </c>
       <c r="H13" t="n">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I13" t="n">
         <v>1</v>
@@ -1452,14 +1452,14 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>$164,242.23</t>
+          <t>$437,979.28</t>
         </is>
       </c>
       <c r="G14" t="n">
         <v>-0.5778520470336813</v>
       </c>
       <c r="H14" t="n">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="I14" t="n">
         <v>1</v>
@@ -1526,14 +1526,14 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>$161,346.58</t>
+          <t>$407,612.42</t>
         </is>
       </c>
       <c r="G15" t="n">
         <v>-1.591651563740375</v>
       </c>
       <c r="H15" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="I15" t="n">
         <v>1</v>
@@ -1600,14 +1600,14 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>$149,698.00</t>
+          <t>$439,114.13</t>
         </is>
       </c>
       <c r="G16" t="n">
         <v>-0.5327190561846336</v>
       </c>
       <c r="H16" t="n">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="I16" t="n">
         <v>1</v>
@@ -1674,14 +1674,14 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>$140,261.89</t>
+          <t>$385,720.19</t>
         </is>
       </c>
       <c r="G17" t="n">
         <v>6.451324737832136</v>
       </c>
       <c r="H17" t="n">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="I17" t="n">
         <v>1</v>
@@ -1748,14 +1748,14 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>$139,649.16</t>
+          <t>$392,763.25</t>
         </is>
       </c>
       <c r="G18" t="n">
         <v>0.717538809957398</v>
       </c>
       <c r="H18" t="n">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="I18" t="n">
         <v>2</v>
@@ -1822,14 +1822,14 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>$128,973.60</t>
+          <t>$386,920.81</t>
         </is>
       </c>
       <c r="G19" t="n">
         <v>-0.699789023367669</v>
       </c>
       <c r="H19" t="n">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="I19" t="n">
         <v>2</v>
@@ -1896,14 +1896,14 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>$137,206.85</t>
+          <t>$431,221.52</t>
         </is>
       </c>
       <c r="G20" t="n">
         <v>16.45400662481288</v>
       </c>
       <c r="H20" t="n">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="I20" t="n">
         <v>2</v>
@@ -1970,14 +1970,14 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>$125,396.86</t>
+          <t>$423,960.81</t>
         </is>
       </c>
       <c r="G21" t="n">
         <v>8.39950986035659</v>
       </c>
       <c r="H21" t="n">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="I21" t="n">
         <v>2</v>
@@ -2044,14 +2044,14 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>$114,500.95</t>
+          <t>$403,479.52</t>
         </is>
       </c>
       <c r="G22" t="n">
         <v>4.208645390631731</v>
       </c>
       <c r="H22" t="n">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="I22" t="n">
         <v>2</v>
@@ -2118,14 +2118,14 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>$114,310.77</t>
+          <t>$379,303.91</t>
         </is>
       </c>
       <c r="G23" t="n">
         <v>5.877671250901471</v>
       </c>
       <c r="H23" t="n">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="I23" t="n">
         <v>3</v>
@@ -2192,14 +2192,14 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>$109,914.90</t>
+          <t>$422,304.63</t>
         </is>
       </c>
       <c r="G24" t="n">
         <v>20.69904339446655</v>
       </c>
       <c r="H24" t="n">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="I24" t="n">
         <v>3</v>
@@ -2266,14 +2266,14 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>$105,599.67</t>
+          <t>$389,051.42</t>
         </is>
       </c>
       <c r="G25" t="n">
         <v>-2.300791655601742</v>
       </c>
       <c r="H25" t="n">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="I25" t="n">
         <v>2</v>
@@ -2340,14 +2340,14 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>$104,776.41</t>
+          <t>$380,503.79</t>
         </is>
       </c>
       <c r="G26" t="n">
         <v>3.563290192005834</v>
       </c>
       <c r="H26" t="n">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="I26" t="n">
         <v>2</v>
@@ -2414,14 +2414,14 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>$99,347.96</t>
+          <t>$375,314.50</t>
         </is>
       </c>
       <c r="G27" t="n">
         <v>5.820872598551052</v>
       </c>
       <c r="H27" t="n">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="I27" t="n">
         <v>2</v>
@@ -2488,14 +2488,14 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>$90,519.72</t>
+          <t>$377,165.50</t>
         </is>
       </c>
       <c r="G28" t="n">
         <v>4.045929734058685</v>
       </c>
       <c r="H28" t="n">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="I28" t="n">
         <v>2</v>
@@ -2562,14 +2562,14 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>$31,187.92</t>
+          <t>$180,196.89</t>
         </is>
       </c>
       <c r="G29" t="n">
         <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
@@ -2636,14 +2636,14 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>$30,464.12</t>
+          <t>$189,554.56</t>
         </is>
       </c>
       <c r="G30" t="n">
         <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="I30" t="n">
         <v>0</v>
@@ -2710,14 +2710,14 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>$27,654.35</t>
+          <t>$190,123.62</t>
         </is>
       </c>
       <c r="G31" t="n">
         <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
@@ -2784,14 +2784,14 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>$25,562.33</t>
+          <t>$161,894.78</t>
         </is>
       </c>
       <c r="G32" t="n">
         <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
@@ -2858,14 +2858,14 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>$17,845.07</t>
+          <t>$129,376.75</t>
         </is>
       </c>
       <c r="G33" t="n">
         <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
@@ -2932,14 +2932,14 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>$15,742.16</t>
+          <t>$131,840.62</t>
         </is>
       </c>
       <c r="G34" t="n">
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
@@ -3006,14 +3006,14 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>$17,267.44</t>
+          <t>$127,347.38</t>
         </is>
       </c>
       <c r="G35" t="n">
         <v>-0.4515208892213129</v>
       </c>
       <c r="H35" t="n">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="I35" t="n">
         <v>0</v>
@@ -3080,14 +3080,14 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>$11,773.76</t>
+          <t>$105,963.88</t>
         </is>
       </c>
       <c r="G36" t="n">
         <v>0.5426377621618689</v>
       </c>
       <c r="H36" t="n">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
@@ -3154,14 +3154,14 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>$11,544.88</t>
+          <t>$53,601.21</t>
         </is>
       </c>
       <c r="G37" t="n">
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
@@ -3228,14 +3228,14 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>$236,321.37</t>
+          <t>$534,832.58</t>
         </is>
       </c>
       <c r="G38" t="n">
         <v>11.90916586882723</v>
       </c>
       <c r="H38" t="n">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="I38" t="n">
         <v>2</v>
@@ -3302,14 +3302,14 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>$323,067.17</t>
+          <t>$735,875.22</t>
         </is>
       </c>
       <c r="G39" t="n">
         <v>4.072620026009845</v>
       </c>
       <c r="H39" t="n">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="I39" t="n">
         <v>1</v>
@@ -3376,14 +3376,14 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>$258,227.46</t>
+          <t>$588,184.78</t>
         </is>
       </c>
       <c r="G40" t="n">
         <v>3.183490902235371</v>
       </c>
       <c r="H40" t="n">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="I40" t="n">
         <v>1</v>
@@ -3450,14 +3450,14 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>$235,021.68</t>
+          <t>$535,327.17</t>
         </is>
       </c>
       <c r="G41" t="n">
         <v>5.920415438575517</v>
       </c>
       <c r="H41" t="n">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="I41" t="n">
         <v>1</v>
@@ -3524,14 +3524,14 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>$333,697.54</t>
+          <t>$760,088.83</t>
         </is>
       </c>
       <c r="G42" t="n">
         <v>2.286868296607728</v>
       </c>
       <c r="H42" t="n">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="I42" t="n">
         <v>1</v>
@@ -3598,14 +3598,14 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>$217,638.07</t>
+          <t>$507,822.17</t>
         </is>
       </c>
       <c r="G43" t="n">
         <v>4.908371795507154</v>
       </c>
       <c r="H43" t="n">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="I43" t="n">
         <v>1</v>
@@ -3672,14 +3672,14 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>$212,730.29</t>
+          <t>$496,370.67</t>
         </is>
       </c>
       <c r="G44" t="n">
         <v>2.169928789775383</v>
       </c>
       <c r="H44" t="n">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="I44" t="n">
         <v>1</v>
@@ -3746,14 +3746,14 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>$184,733.52</t>
+          <t>$451,570.83</t>
         </is>
       </c>
       <c r="G45" t="n">
         <v>2.918686683213843</v>
       </c>
       <c r="H45" t="n">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="I45" t="n">
         <v>1</v>
@@ -3820,14 +3820,14 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>$189,592.05</t>
+          <t>$479,556.35</t>
         </is>
       </c>
       <c r="G46" t="n">
         <v>-0.484963430661035</v>
       </c>
       <c r="H46" t="n">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="I46" t="n">
         <v>1</v>
@@ -3894,14 +3894,14 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>$166,913.42</t>
+          <t>$562,234.68</t>
         </is>
       </c>
       <c r="G47" t="n">
         <v>22.38235653420247</v>
       </c>
       <c r="H47" t="n">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="I47" t="n">
         <v>2</v>
@@ -3968,14 +3968,14 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>$154,171.70</t>
+          <t>$535,543.79</t>
         </is>
       </c>
       <c r="G48" t="n">
         <v>11.45138163550831</v>
       </c>
       <c r="H48" t="n">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="I48" t="n">
         <v>2</v>
@@ -4042,14 +4042,14 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>$187,422.14</t>
+          <t>$691,119.12</t>
         </is>
       </c>
       <c r="G49" t="n">
         <v>2.152455627674896</v>
       </c>
       <c r="H49" t="n">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="I49" t="n">
         <v>1</v>
@@ -4116,14 +4116,14 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>$161,154.70</t>
+          <t>$656,129.86</t>
         </is>
       </c>
       <c r="G50" t="n">
         <v>1.375171704904234</v>
       </c>
       <c r="H50" t="n">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="I50" t="n">
         <v>1</v>
@@ -4190,14 +4190,14 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>$163,274.93</t>
+          <t>$676,424.71</t>
         </is>
       </c>
       <c r="G51" t="n">
         <v>3.487224531164169</v>
       </c>
       <c r="H51" t="n">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="I51" t="n">
         <v>1</v>
@@ -4264,14 +4264,14 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>$163,234.65</t>
+          <t>$664,598.21</t>
         </is>
       </c>
       <c r="G52" t="n">
         <v>1.41833309598979</v>
       </c>
       <c r="H52" t="n">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="I52" t="n">
         <v>1</v>
@@ -4338,14 +4338,14 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>$140,728.62</t>
+          <t>$603,122.64</t>
         </is>
       </c>
       <c r="G53" t="n">
         <v>5.831673183741236</v>
       </c>
       <c r="H53" t="n">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="I53" t="n">
         <v>1</v>
@@ -4412,14 +4412,14 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>$132,663.78</t>
+          <t>$530,655.12</t>
         </is>
       </c>
       <c r="G54" t="n">
         <v>5.673864923098594</v>
       </c>
       <c r="H54" t="n">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="I54" t="n">
         <v>1</v>
@@ -4486,14 +4486,14 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>$141,755.37</t>
+          <t>$472,517.90</t>
         </is>
       </c>
       <c r="G55" t="n">
         <v>6.127888930588269</v>
       </c>
       <c r="H55" t="n">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="I55" t="n">
         <v>1</v>
@@ -4560,14 +4560,14 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>$322,594.67</t>
+          <t>$806,486.68</t>
         </is>
       </c>
       <c r="G56" t="n">
         <v>13.89307093894973</v>
       </c>
       <c r="H56" t="n">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="I56" t="n">
         <v>1</v>
@@ -4634,14 +4634,14 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>$254,570.43</t>
+          <t>$649,154.60</t>
         </is>
       </c>
       <c r="G57" t="n">
         <v>16.45033448118522</v>
       </c>
       <c r="H57" t="n">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="I57" t="n">
         <v>1</v>
@@ -4708,14 +4708,14 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>$246,347.78</t>
+          <t>$660,659.95</t>
         </is>
       </c>
       <c r="G58" t="n">
         <v>16.48548059966759</v>
       </c>
       <c r="H58" t="n">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="I58" t="n">
         <v>1</v>
@@ -4782,14 +4782,14 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>$231,165.03</t>
+          <t>$638,455.81</t>
         </is>
       </c>
       <c r="G59" t="n">
         <v>15.26870510186333</v>
       </c>
       <c r="H59" t="n">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="I59" t="n">
         <v>1</v>
@@ -4856,14 +4856,14 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>$205,141.77</t>
+          <t>$615,425.30</t>
         </is>
       </c>
       <c r="G60" t="n">
         <v>12.55271687725545</v>
       </c>
       <c r="H60" t="n">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="I60" t="n">
         <v>1</v>
@@ -4930,14 +4930,14 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>$207,190.12</t>
+          <t>$546,981.92</t>
         </is>
       </c>
       <c r="G61" t="n">
         <v>6.796688343921861</v>
       </c>
       <c r="H61" t="n">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="I61" t="n">
         <v>3</v>
@@ -5004,14 +5004,14 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>$190,681.76</t>
+          <t>$500,539.62</t>
         </is>
       </c>
       <c r="G62" t="n">
         <v>6.624333937597847</v>
       </c>
       <c r="H62" t="n">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="I62" t="n">
         <v>3</v>
@@ -5078,14 +5078,14 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>$204,178.80</t>
+          <t>$510,447.00</t>
         </is>
       </c>
       <c r="G63" t="n">
         <v>9.240503258255346</v>
       </c>
       <c r="H63" t="n">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="I63" t="n">
         <v>2</v>
@@ -5152,14 +5152,14 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>$216,472.03</t>
+          <t>$448,406.36</t>
         </is>
       </c>
       <c r="G64" t="n">
         <v>9.64443770629606</v>
       </c>
       <c r="H64" t="n">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="I64" t="n">
         <v>2</v>
@@ -5226,14 +5226,14 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>$175,530.71</t>
+          <t>$678,718.73</t>
         </is>
       </c>
       <c r="G65" t="n">
         <v>28.62134417781897</v>
       </c>
       <c r="H65" t="n">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="I65" t="n">
         <v>1</v>
@@ -5300,14 +5300,14 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>$172,630.88</t>
+          <t>$743,640.69</t>
         </is>
       </c>
       <c r="G66" t="n">
         <v>36.87306131817796</v>
       </c>
       <c r="H66" t="n">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="I66" t="n">
         <v>1</v>
@@ -5374,14 +5374,14 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>$183,280.44</t>
+          <t>$746,213.21</t>
         </is>
       </c>
       <c r="G67" t="n">
         <v>10.58742756881531</v>
       </c>
       <c r="H67" t="n">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="I67" t="n">
         <v>1</v>
@@ -5448,14 +5448,14 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>$186,990.62</t>
+          <t>$805,498.08</t>
         </is>
       </c>
       <c r="G68" t="n">
         <v>22.21328953179948</v>
       </c>
       <c r="H68" t="n">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="I68" t="n">
         <v>1</v>
@@ -5522,14 +5522,14 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>$165,127.02</t>
+          <t>$673,210.15</t>
         </is>
       </c>
       <c r="G69" t="n">
         <v>30.27751752453115</v>
       </c>
       <c r="H69" t="n">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="I69" t="n">
         <v>1</v>
@@ -5596,14 +5596,14 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>$150,836.75</t>
+          <t>$703,904.83</t>
         </is>
       </c>
       <c r="G70" t="n">
         <v>42.06602230083659</v>
       </c>
       <c r="H70" t="n">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="I70" t="n">
         <v>1</v>
@@ -5670,14 +5670,14 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>$168,570.48</t>
+          <t>$674,281.93</t>
         </is>
       </c>
       <c r="G71" t="n">
         <v>23.04041887099578</v>
       </c>
       <c r="H71" t="n">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="I71" t="n">
         <v>1</v>
@@ -5744,14 +5744,14 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>$177,741.36</t>
+          <t>$765,655.08</t>
         </is>
       </c>
       <c r="G72" t="n">
         <v>16.25192625399909</v>
       </c>
       <c r="H72" t="n">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="I72" t="n">
         <v>1</v>
@@ -5818,14 +5818,14 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>$160,390.80</t>
+          <t>$598,792.33</t>
         </is>
       </c>
       <c r="G73" t="n">
         <v>23.34664182407145</v>
       </c>
       <c r="H73" t="n">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="I73" t="n">
         <v>1</v>
@@ -5892,14 +5892,14 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>$109,399.62</t>
+          <t>$477,380.18</t>
         </is>
       </c>
       <c r="G74" t="n">
         <v>22.2149363705162</v>
       </c>
       <c r="H74" t="n">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="I74" t="n">
         <v>1</v>
@@ -5966,14 +5966,14 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>$117,091.69</t>
+          <t>$405,917.87</t>
         </is>
       </c>
       <c r="G75" t="n">
         <v>8.403600695575854</v>
       </c>
       <c r="H75" t="n">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="I75" t="n">
         <v>1</v>
@@ -6040,14 +6040,14 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>$130,986.09</t>
+          <t>$416,073.47</t>
         </is>
       </c>
       <c r="G76" t="n">
         <v>4.956564232363373</v>
       </c>
       <c r="H76" t="n">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="I76" t="n">
         <v>2</v>
@@ -6114,14 +6114,14 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>$117,651.36</t>
+          <t>$385,635.00</t>
         </is>
       </c>
       <c r="G77" t="n">
         <v>2.146422999295534</v>
       </c>
       <c r="H77" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="I77" t="n">
         <v>1</v>
@@ -6188,14 +6188,14 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>$107,908.60</t>
+          <t>$386,199.21</t>
         </is>
       </c>
       <c r="G78" t="n">
         <v>4.774206112607551</v>
       </c>
       <c r="H78" t="n">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="I78" t="n">
         <v>1</v>
@@ -6262,14 +6262,14 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>$114,179.27</t>
+          <t>$332,609.17</t>
         </is>
       </c>
       <c r="G79" t="n">
         <v>0.9525430747746637</v>
       </c>
       <c r="H79" t="n">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="I79" t="n">
         <v>1</v>
@@ -6336,14 +6336,14 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>$115,021.48</t>
+          <t>$294,455.00</t>
         </is>
       </c>
       <c r="G80" t="n">
         <v>0.3131709768895077</v>
       </c>
       <c r="H80" t="n">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="I80" t="n">
         <v>1</v>
@@ -6410,14 +6410,14 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>$127,199.44</t>
+          <t>$315,454.60</t>
         </is>
       </c>
       <c r="G81" t="n">
         <v>1.512494793228566</v>
       </c>
       <c r="H81" t="n">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="I81" t="n">
         <v>1</v>
@@ -6484,14 +6484,14 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>$114,572.58</t>
+          <t>$286,431.46</t>
         </is>
       </c>
       <c r="G82" t="n">
         <v>2.218000234203791</v>
       </c>
       <c r="H82" t="n">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="I82" t="n">
         <v>2</v>
@@ -6558,14 +6558,14 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>$180,080.74</t>
+          <t>$336,672.70</t>
         </is>
       </c>
       <c r="G83" t="n">
         <v>3.552015814094763</v>
       </c>
       <c r="H83" t="n">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="I83" t="n">
         <v>3</v>
@@ -6632,14 +6632,14 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>$181,013.60</t>
+          <t>$354,157.04</t>
         </is>
       </c>
       <c r="G84" t="n">
         <v>0.6828848464670303</v>
       </c>
       <c r="H84" t="n">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I84" t="n">
         <v>1</v>
@@ -6706,14 +6706,14 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>$180,684.08</t>
+          <t>$354,140.80</t>
         </is>
       </c>
       <c r="G85" t="n">
         <v>1.056612962979696</v>
       </c>
       <c r="H85" t="n">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="I85" t="n">
         <v>2</v>
@@ -6780,14 +6780,14 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>$180,645.98</t>
+          <t>$361,291.96</t>
         </is>
       </c>
       <c r="G86" t="n">
         <v>0.6650393662466193</v>
       </c>
       <c r="H86" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="I86" t="n">
         <v>2</v>
@@ -6854,14 +6854,14 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>$182,284.41</t>
+          <t>$444,318.25</t>
         </is>
       </c>
       <c r="G87" t="n">
         <v>1.125231464158855</v>
       </c>
       <c r="H87" t="n">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="I87" t="n">
         <v>1</v>
@@ -6928,14 +6928,14 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>$150,899.97</t>
+          <t>$372,219.93</t>
         </is>
       </c>
       <c r="G88" t="n">
         <v>1.26253313677093</v>
       </c>
       <c r="H88" t="n">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="I88" t="n">
         <v>1</v>
@@ -7002,14 +7002,14 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>$135,049.59</t>
+          <t>$416,402.92</t>
         </is>
       </c>
       <c r="G89" t="n">
         <v>1.811495876890072</v>
       </c>
       <c r="H89" t="n">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="I89" t="n">
         <v>1</v>
@@ -7076,14 +7076,14 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>$148,361.39</t>
+          <t>$433,671.77</t>
         </is>
       </c>
       <c r="G90" t="n">
         <v>3.318428524373183</v>
       </c>
       <c r="H90" t="n">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="I90" t="n">
         <v>1</v>
@@ -7150,14 +7150,14 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>$133,979.74</t>
+          <t>$391,633.08</t>
         </is>
       </c>
       <c r="G91" t="n">
         <v>4.402518448390664</v>
       </c>
       <c r="H91" t="n">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="I91" t="n">
         <v>1</v>
@@ -7224,14 +7224,14 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>$120,884.55</t>
+          <t>$295,495.56</t>
         </is>
       </c>
       <c r="G92" t="n">
         <v>7.807979815451257</v>
       </c>
       <c r="H92" t="n">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="I92" t="n">
         <v>1</v>
@@ -7298,14 +7298,14 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>$120,062.63</t>
+          <t>$306,826.72</t>
         </is>
       </c>
       <c r="G93" t="n">
         <v>-1.223812535522674</v>
       </c>
       <c r="H93" t="n">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="I93" t="n">
         <v>1</v>
@@ -7372,14 +7372,14 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>$123,349.73</t>
+          <t>$308,374.33</t>
         </is>
       </c>
       <c r="G94" t="n">
         <v>-1.569519584602984</v>
       </c>
       <c r="H94" t="n">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="I94" t="n">
         <v>1</v>
@@ -7446,14 +7446,14 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>$115,852.52</t>
+          <t>$318,594.44</t>
         </is>
       </c>
       <c r="G95" t="n">
         <v>0.09105561518160529</v>
       </c>
       <c r="H95" t="n">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="I95" t="n">
         <v>1</v>
@@ -7520,14 +7520,14 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>$132,413.33</t>
+          <t>$320,579.63</t>
         </is>
       </c>
       <c r="G96" t="n">
         <v>2.39970231552617</v>
       </c>
       <c r="H96" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="I96" t="n">
         <v>1</v>
@@ -7594,14 +7594,14 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>$114,250.80</t>
+          <t>$294,646.79</t>
         </is>
       </c>
       <c r="G97" t="n">
         <v>0.6458566179773856</v>
       </c>
       <c r="H97" t="n">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="I97" t="n">
         <v>2</v>
@@ -7668,14 +7668,14 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>$99,851.31</t>
+          <t>$268,021.95</t>
         </is>
       </c>
       <c r="G98" t="n">
         <v>3.97355538637154</v>
       </c>
       <c r="H98" t="n">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="I98" t="n">
         <v>1</v>
@@ -7742,14 +7742,14 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>$102,372.77</t>
+          <t>$295,743.56</t>
         </is>
       </c>
       <c r="G99" t="n">
         <v>4.500335313026451</v>
       </c>
       <c r="H99" t="n">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="I99" t="n">
         <v>1</v>
@@ -7816,14 +7816,14 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>$99,936.02</t>
+          <t>$294,256.06</t>
         </is>
       </c>
       <c r="G100" t="n">
         <v>4.924632911358946</v>
       </c>
       <c r="H100" t="n">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="I100" t="n">
         <v>2</v>
@@ -7890,14 +7890,14 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>$174,507.48</t>
+          <t>$523,522.44</t>
         </is>
       </c>
       <c r="G101" t="n">
         <v>3.430738828559192</v>
       </c>
       <c r="H101" t="n">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="I101" t="n">
         <v>1</v>
@@ -7964,14 +7964,14 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>$172,573.73</t>
+          <t>$527,872.59</t>
         </is>
       </c>
       <c r="G102" t="n">
         <v>2.886126487296288</v>
       </c>
       <c r="H102" t="n">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="I102" t="n">
         <v>1</v>
@@ -8038,14 +8038,14 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>$167,108.58</t>
+          <t>$543,102.88</t>
         </is>
       </c>
       <c r="G103" t="n">
         <v>0.4729818683062578</v>
       </c>
       <c r="H103" t="n">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="I103" t="n">
         <v>1</v>
@@ -8112,14 +8112,14 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>$164,619.52</t>
+          <t>$535,013.44</t>
         </is>
       </c>
       <c r="G104" t="n">
         <v>2.639643163168215</v>
       </c>
       <c r="H104" t="n">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="I104" t="n">
         <v>1</v>
@@ -8186,14 +8186,14 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>$133,178.82</t>
+          <t>$512,226.23</t>
         </is>
       </c>
       <c r="G105" t="n">
         <v>4.269191602688776</v>
       </c>
       <c r="H105" t="n">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="I105" t="n">
         <v>1</v>
@@ -8260,14 +8260,14 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>$124,768.38</t>
+          <t>$479,878.38</t>
         </is>
       </c>
       <c r="G106" t="n">
         <v>3.371978220763947</v>
       </c>
       <c r="H106" t="n">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="I106" t="n">
         <v>1</v>
@@ -8334,14 +8334,14 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>$118,617.67</t>
+          <t>$447,097.38</t>
         </is>
       </c>
       <c r="G107" t="n">
         <v>4.179199988438244</v>
       </c>
       <c r="H107" t="n">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="I107" t="n">
         <v>1</v>
@@ -8408,14 +8408,14 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>$115,722.25</t>
+          <t>$396,762.00</t>
         </is>
       </c>
       <c r="G108" t="n">
         <v>4.306909431850833</v>
       </c>
       <c r="H108" t="n">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="I108" t="n">
         <v>1</v>
@@ -8482,14 +8482,14 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>$111,776.74</t>
+          <t>$342,782.00</t>
         </is>
       </c>
       <c r="G109" t="n">
         <v>3.368173552481363</v>
       </c>
       <c r="H109" t="n">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="I109" t="n">
         <v>1</v>
@@ -8556,14 +8556,14 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>$82,098.56</t>
+          <t>$307,869.58</t>
         </is>
       </c>
       <c r="G110" t="n">
         <v>4.029481097921604</v>
       </c>
       <c r="H110" t="n">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="I110" t="n">
         <v>1</v>
@@ -8630,14 +8630,14 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>$90,577.73</t>
+          <t>$301,925.75</t>
         </is>
       </c>
       <c r="G111" t="n">
         <v>0.8259152567587671</v>
       </c>
       <c r="H111" t="n">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="I111" t="n">
         <v>1</v>
@@ -8704,14 +8704,14 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>$75,656.15</t>
+          <t>$238,607.85</t>
         </is>
       </c>
       <c r="G112" t="n">
         <v>-1.005482442707732</v>
       </c>
       <c r="H112" t="n">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="I112" t="n">
         <v>2</v>
@@ -8778,14 +8778,14 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>$79,383.17</t>
+          <t>$285,779.40</t>
         </is>
       </c>
       <c r="G113" t="n">
         <v>0.04320220421765879</v>
       </c>
       <c r="H113" t="n">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="I113" t="n">
         <v>2</v>
@@ -8852,14 +8852,14 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>$73,752.89</t>
+          <t>$303,206.33</t>
         </is>
       </c>
       <c r="G114" t="n">
         <v>0.5099310810350267</v>
       </c>
       <c r="H114" t="n">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="I114" t="n">
         <v>1</v>
@@ -8926,14 +8926,14 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>$82,516.17</t>
+          <t>$275,053.89</t>
         </is>
       </c>
       <c r="G115" t="n">
         <v>1.27917761569955</v>
       </c>
       <c r="H115" t="n">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="I115" t="n">
         <v>1</v>
@@ -9000,14 +9000,14 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>$99,322.27</t>
+          <t>$273,136.25</t>
         </is>
       </c>
       <c r="G116" t="n">
         <v>0.5779935837883108</v>
       </c>
       <c r="H116" t="n">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="I116" t="n">
         <v>1</v>
@@ -9074,14 +9074,14 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>$87,196.89</t>
+          <t>$261,590.67</t>
         </is>
       </c>
       <c r="G117" t="n">
         <v>0.757098239998369</v>
       </c>
       <c r="H117" t="n">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="I117" t="n">
         <v>1</v>
@@ -9148,14 +9148,14 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>$82,442.50</t>
+          <t>$261,067.92</t>
         </is>
       </c>
       <c r="G118" t="n">
         <v>0.2288440268576344</v>
       </c>
       <c r="H118" t="n">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="I118" t="n">
         <v>1</v>
@@ -9533,47 +9533,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$109,399.62</t>
+          <t>$477,380.18</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$117,091.69</t>
+          <t>$405,917.87</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$130,986.09</t>
+          <t>$416,073.47</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$117,651.36</t>
+          <t>$385,635.00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$107,908.60</t>
+          <t>$386,199.21</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>$114,179.27</t>
+          <t>$332,609.17</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>$115,021.48</t>
+          <t>$294,455.00</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>$127,199.44</t>
+          <t>$315,454.60</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>$114,572.58</t>
+          <t>$286,431.46</t>
         </is>
       </c>
     </row>
@@ -9617,42 +9617,32 @@
           <t>Total Reported Employees</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Title Group</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Base Compensation</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Other Comp</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Total Comp</t>
-        </is>
+      <c r="B9" t="n">
+        <v>11</v>
+      </c>
+      <c r="C9" t="n">
+        <v>15</v>
+      </c>
+      <c r="D9" t="n">
+        <v>17</v>
+      </c>
+      <c r="E9" t="n">
+        <v>18</v>
+      </c>
+      <c r="F9" t="n">
+        <v>19</v>
+      </c>
+      <c r="G9" t="n">
+        <v>23</v>
+      </c>
+      <c r="H9" t="n">
+        <v>25</v>
+      </c>
+      <c r="I9" t="n">
+        <v>25</v>
+      </c>
+      <c r="J9" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="11">
@@ -15518,47 +15508,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$180,080.74</t>
+          <t>$336,672.70</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$181,013.60</t>
+          <t>$354,157.04</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$180,684.08</t>
+          <t>$354,140.80</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$180,645.98</t>
+          <t>$361,291.96</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$182,284.41</t>
+          <t>$444,318.25</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>$150,899.97</t>
+          <t>$372,219.93</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>$135,049.59</t>
+          <t>$416,402.92</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>$148,361.39</t>
+          <t>$433,671.77</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>$133,979.74</t>
+          <t>$391,633.08</t>
         </is>
       </c>
     </row>
@@ -15602,42 +15592,32 @@
           <t>Total Reported Employees</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Title Group</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Base Compensation</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Other Comp</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Total Comp</t>
-        </is>
+      <c r="B9" t="n">
+        <v>23</v>
+      </c>
+      <c r="C9" t="n">
+        <v>23</v>
+      </c>
+      <c r="D9" t="n">
+        <v>25</v>
+      </c>
+      <c r="E9" t="n">
+        <v>24</v>
+      </c>
+      <c r="F9" t="n">
+        <v>16</v>
+      </c>
+      <c r="G9" t="n">
+        <v>15</v>
+      </c>
+      <c r="H9" t="n">
+        <v>12</v>
+      </c>
+      <c r="I9" t="n">
+        <v>13</v>
+      </c>
+      <c r="J9" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -21100,47 +21080,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$120,884.55</t>
+          <t>$295,495.56</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$120,062.63</t>
+          <t>$306,826.72</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$123,349.73</t>
+          <t>$308,374.33</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$115,852.52</t>
+          <t>$318,594.44</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$132,413.33</t>
+          <t>$320,579.63</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>$114,250.80</t>
+          <t>$294,646.79</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>$99,851.31</t>
+          <t>$268,021.95</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>$102,372.77</t>
+          <t>$295,743.56</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>$99,936.02</t>
+          <t>$294,256.06</t>
         </is>
       </c>
     </row>
@@ -21184,42 +21164,32 @@
           <t>Total Reported Employees</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Title Group</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Base Compensation</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Other Comp</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Total Comp</t>
-        </is>
+      <c r="B9" t="n">
+        <v>18</v>
+      </c>
+      <c r="C9" t="n">
+        <v>18</v>
+      </c>
+      <c r="D9" t="n">
+        <v>18</v>
+      </c>
+      <c r="E9" t="n">
+        <v>16</v>
+      </c>
+      <c r="F9" t="n">
+        <v>19</v>
+      </c>
+      <c r="G9" t="n">
+        <v>19</v>
+      </c>
+      <c r="H9" t="n">
+        <v>19</v>
+      </c>
+      <c r="I9" t="n">
+        <v>18</v>
+      </c>
+      <c r="J9" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="11">
@@ -26651,47 +26621,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$174,507.48</t>
+          <t>$523,522.44</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$172,573.73</t>
+          <t>$527,872.59</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$167,108.58</t>
+          <t>$543,102.88</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$164,619.52</t>
+          <t>$535,013.44</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$133,178.82</t>
+          <t>$512,226.23</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>$124,768.38</t>
+          <t>$479,878.38</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>$118,617.67</t>
+          <t>$447,097.38</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>$115,722.25</t>
+          <t>$396,762.00</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>$111,776.74</t>
+          <t>$342,782.00</t>
         </is>
       </c>
     </row>
@@ -26735,42 +26705,32 @@
           <t>Total Reported Employees</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Title Group</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Base Compensation</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Other Comp</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Total Comp</t>
-        </is>
+      <c r="B9" t="n">
+        <v>18</v>
+      </c>
+      <c r="C9" t="n">
+        <v>17</v>
+      </c>
+      <c r="D9" t="n">
+        <v>16</v>
+      </c>
+      <c r="E9" t="n">
+        <v>16</v>
+      </c>
+      <c r="F9" t="n">
+        <v>13</v>
+      </c>
+      <c r="G9" t="n">
+        <v>13</v>
+      </c>
+      <c r="H9" t="n">
+        <v>13</v>
+      </c>
+      <c r="I9" t="n">
+        <v>14</v>
+      </c>
+      <c r="J9" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="11">
@@ -31334,47 +31294,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$82,098.56</t>
+          <t>$307,869.58</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$90,577.73</t>
+          <t>$301,925.75</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$75,656.15</t>
+          <t>$238,607.85</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$79,383.17</t>
+          <t>$285,779.40</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$73,752.89</t>
+          <t>$303,206.33</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>$82,516.17</t>
+          <t>$275,053.89</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>$99,322.27</t>
+          <t>$273,136.25</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>$87,196.89</t>
+          <t>$261,590.67</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>$82,442.50</t>
+          <t>$261,067.92</t>
         </is>
       </c>
     </row>
@@ -31418,42 +31378,32 @@
           <t>Total Reported Employees</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Title Group</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Base Compensation</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Other Comp</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Total Comp</t>
-        </is>
+      <c r="B9" t="n">
+        <v>12</v>
+      </c>
+      <c r="C9" t="n">
+        <v>12</v>
+      </c>
+      <c r="D9" t="n">
+        <v>13</v>
+      </c>
+      <c r="E9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F9" t="n">
+        <v>9</v>
+      </c>
+      <c r="G9" t="n">
+        <v>9</v>
+      </c>
+      <c r="H9" t="n">
+        <v>12</v>
+      </c>
+      <c r="I9" t="n">
+        <v>12</v>
+      </c>
+      <c r="J9" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -34963,47 +34913,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$175,637.81</t>
+          <t>$381,558.00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$164,243.46</t>
+          <t>$356,804.76</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$178,941.12</t>
+          <t>$346,337.65</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$178,160.92</t>
+          <t>$349,723.30</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$169,000.15</t>
+          <t>$338,000.30</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>$182,967.22</t>
+          <t>$351,860.04</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>$166,855.72</t>
+          <t>$333,711.44</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>$154,768.69</t>
+          <t>$315,269.56</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>$156,988.46</t>
+          <t>$301,900.88</t>
         </is>
       </c>
     </row>
@@ -35047,42 +34997,32 @@
           <t>Total Reported Employees</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Title Group</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Base Compensation</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Other Comp</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Total Comp</t>
-        </is>
+      <c r="B9" t="n">
+        <v>29</v>
+      </c>
+      <c r="C9" t="n">
+        <v>29</v>
+      </c>
+      <c r="D9" t="n">
+        <v>31</v>
+      </c>
+      <c r="E9" t="n">
+        <v>27</v>
+      </c>
+      <c r="F9" t="n">
+        <v>27</v>
+      </c>
+      <c r="G9" t="n">
+        <v>26</v>
+      </c>
+      <c r="H9" t="n">
+        <v>27</v>
+      </c>
+      <c r="I9" t="n">
+        <v>27</v>
+      </c>
+      <c r="J9" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="11">
@@ -43180,47 +43120,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$177,885.33</t>
+          <t>$449,394.53</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$149,100.25</t>
+          <t>$397,600.67</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$175,711.54</t>
+          <t>$496,126.71</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$164,242.23</t>
+          <t>$437,979.28</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$161,346.58</t>
+          <t>$407,612.42</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>$149,698.00</t>
+          <t>$439,114.13</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>$140,261.89</t>
+          <t>$385,720.19</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>$139,649.16</t>
+          <t>$392,763.25</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>$128,973.60</t>
+          <t>$386,920.81</t>
         </is>
       </c>
     </row>
@@ -43264,42 +43204,32 @@
           <t>Total Reported Employees</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Title Group</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Base Compensation</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Other Comp</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Total Comp</t>
-        </is>
+      <c r="B9" t="n">
+        <v>19</v>
+      </c>
+      <c r="C9" t="n">
+        <v>18</v>
+      </c>
+      <c r="D9" t="n">
+        <v>17</v>
+      </c>
+      <c r="E9" t="n">
+        <v>18</v>
+      </c>
+      <c r="F9" t="n">
+        <v>19</v>
+      </c>
+      <c r="G9" t="n">
+        <v>15</v>
+      </c>
+      <c r="H9" t="n">
+        <v>16</v>
+      </c>
+      <c r="I9" t="n">
+        <v>16</v>
+      </c>
+      <c r="J9" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="11">
@@ -48452,47 +48382,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$137,206.85</t>
+          <t>$431,221.52</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$125,396.86</t>
+          <t>$423,960.81</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$114,500.95</t>
+          <t>$403,479.52</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$114,310.77</t>
+          <t>$379,303.91</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$109,914.90</t>
+          <t>$422,304.63</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>$105,599.67</t>
+          <t>$389,051.42</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>$104,776.41</t>
+          <t>$380,503.79</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>$99,347.96</t>
+          <t>$375,314.50</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>$90,519.72</t>
+          <t>$377,165.50</t>
         </is>
       </c>
     </row>
@@ -48536,42 +48466,32 @@
           <t>Total Reported Employees</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Title Group</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Base Compensation</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Other Comp</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Total Comp</t>
-        </is>
+      <c r="B9" t="n">
+        <v>21</v>
+      </c>
+      <c r="C9" t="n">
+        <v>21</v>
+      </c>
+      <c r="D9" t="n">
+        <v>21</v>
+      </c>
+      <c r="E9" t="n">
+        <v>22</v>
+      </c>
+      <c r="F9" t="n">
+        <v>19</v>
+      </c>
+      <c r="G9" t="n">
+        <v>19</v>
+      </c>
+      <c r="H9" t="n">
+        <v>19</v>
+      </c>
+      <c r="I9" t="n">
+        <v>18</v>
+      </c>
+      <c r="J9" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="11">
@@ -54468,47 +54388,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$31,187.92</t>
+          <t>$180,196.89</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$30,464.12</t>
+          <t>$189,554.56</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$27,654.35</t>
+          <t>$190,123.62</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$25,562.33</t>
+          <t>$161,894.78</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$17,845.07</t>
+          <t>$129,376.75</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>$15,742.16</t>
+          <t>$131,840.62</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>$17,267.44</t>
+          <t>$127,347.38</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>$11,773.76</t>
+          <t>$105,963.88</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>$11,544.88</t>
+          <t>$53,601.21</t>
         </is>
       </c>
     </row>
@@ -54552,42 +54472,32 @@
           <t>Total Reported Employees</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Title Group</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Base Compensation</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Other Comp</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Total Comp</t>
-        </is>
+      <c r="B9" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="D9" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9</v>
+      </c>
+      <c r="F9" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8</v>
+      </c>
+      <c r="H9" t="n">
+        <v>8</v>
+      </c>
+      <c r="I9" t="n">
+        <v>8</v>
+      </c>
+      <c r="J9" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="11">
@@ -57477,47 +57387,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$236,321.37</t>
+          <t>$534,832.58</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$323,067.17</t>
+          <t>$735,875.22</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$258,227.46</t>
+          <t>$588,184.78</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$235,021.68</t>
+          <t>$535,327.17</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$333,697.54</t>
+          <t>$760,088.83</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>$217,638.07</t>
+          <t>$507,822.17</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>$212,730.29</t>
+          <t>$496,370.67</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>$184,733.52</t>
+          <t>$451,570.83</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>$189,592.05</t>
+          <t>$479,556.35</t>
         </is>
       </c>
     </row>
@@ -57561,42 +57471,32 @@
           <t>Total Reported Employees</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Title Group</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Base Compensation</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Other Comp</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Total Comp</t>
-        </is>
+      <c r="B9" t="n">
+        <v>19</v>
+      </c>
+      <c r="C9" t="n">
+        <v>18</v>
+      </c>
+      <c r="D9" t="n">
+        <v>18</v>
+      </c>
+      <c r="E9" t="n">
+        <v>18</v>
+      </c>
+      <c r="F9" t="n">
+        <v>18</v>
+      </c>
+      <c r="G9" t="n">
+        <v>18</v>
+      </c>
+      <c r="H9" t="n">
+        <v>18</v>
+      </c>
+      <c r="I9" t="n">
+        <v>18</v>
+      </c>
+      <c r="J9" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="11">
@@ -62997,47 +62897,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$166,913.42</t>
+          <t>$562,234.68</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$154,171.70</t>
+          <t>$535,543.79</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$187,422.14</t>
+          <t>$691,119.12</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$161,154.70</t>
+          <t>$656,129.86</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$163,274.93</t>
+          <t>$676,424.71</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>$163,234.65</t>
+          <t>$664,598.21</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>$140,728.62</t>
+          <t>$603,122.64</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>$132,663.78</t>
+          <t>$530,655.12</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>$141,755.37</t>
+          <t>$472,517.90</t>
         </is>
       </c>
     </row>
@@ -63081,42 +62981,32 @@
           <t>Total Reported Employees</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Title Group</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Base Compensation</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Other Comp</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Total Comp</t>
-        </is>
+      <c r="B9" t="n">
+        <v>19</v>
+      </c>
+      <c r="C9" t="n">
+        <v>19</v>
+      </c>
+      <c r="D9" t="n">
+        <v>16</v>
+      </c>
+      <c r="E9" t="n">
+        <v>14</v>
+      </c>
+      <c r="F9" t="n">
+        <v>14</v>
+      </c>
+      <c r="G9" t="n">
+        <v>14</v>
+      </c>
+      <c r="H9" t="n">
+        <v>14</v>
+      </c>
+      <c r="I9" t="n">
+        <v>16</v>
+      </c>
+      <c r="J9" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="11">
@@ -68052,47 +67942,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$322,594.67</t>
+          <t>$806,486.68</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$254,570.43</t>
+          <t>$649,154.60</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$246,347.78</t>
+          <t>$660,659.95</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$231,165.03</t>
+          <t>$638,455.81</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$205,141.77</t>
+          <t>$615,425.30</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>$207,190.12</t>
+          <t>$546,981.92</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>$190,681.76</t>
+          <t>$500,539.62</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>$204,178.80</t>
+          <t>$510,447.00</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>$216,472.03</t>
+          <t>$448,406.36</t>
         </is>
       </c>
     </row>
@@ -68136,42 +68026,32 @@
           <t>Total Reported Employees</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Title Group</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Base Compensation</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Other Comp</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Total Comp</t>
-        </is>
+      <c r="B9" t="n">
+        <v>22</v>
+      </c>
+      <c r="C9" t="n">
+        <v>20</v>
+      </c>
+      <c r="D9" t="n">
+        <v>22</v>
+      </c>
+      <c r="E9" t="n">
+        <v>21</v>
+      </c>
+      <c r="F9" t="n">
+        <v>20</v>
+      </c>
+      <c r="G9" t="n">
+        <v>25</v>
+      </c>
+      <c r="H9" t="n">
+        <v>24</v>
+      </c>
+      <c r="I9" t="n">
+        <v>24</v>
+      </c>
+      <c r="J9" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="11">
@@ -74936,47 +74816,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$175,530.71</t>
+          <t>$678,718.73</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$172,630.88</t>
+          <t>$743,640.69</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$183,280.44</t>
+          <t>$746,213.21</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$186,990.62</t>
+          <t>$805,498.08</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$165,127.02</t>
+          <t>$673,210.15</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>$150,836.75</t>
+          <t>$703,904.83</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>$168,570.48</t>
+          <t>$674,281.93</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>$177,741.36</t>
+          <t>$765,655.08</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>$160,390.80</t>
+          <t>$598,792.33</t>
         </is>
       </c>
     </row>
@@ -75020,42 +74900,32 @@
           <t>Total Reported Employees</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Title Group</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Base Compensation</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Other Comp</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Total Comp</t>
-        </is>
+      <c r="B9" t="n">
+        <v>15</v>
+      </c>
+      <c r="C9" t="n">
+        <v>13</v>
+      </c>
+      <c r="D9" t="n">
+        <v>14</v>
+      </c>
+      <c r="E9" t="n">
+        <v>13</v>
+      </c>
+      <c r="F9" t="n">
+        <v>13</v>
+      </c>
+      <c r="G9" t="n">
+        <v>12</v>
+      </c>
+      <c r="H9" t="n">
+        <v>14</v>
+      </c>
+      <c r="I9" t="n">
+        <v>13</v>
+      </c>
+      <c r="J9" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="11">

</xml_diff>